<commit_message>
test plan: sheet reorganized, added some test cases
</commit_message>
<xml_diff>
--- a/Test/C780_Binary_Library_Test_Plan.xlsx
+++ b/Test/C780_Binary_Library_Test_Plan.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\hwfwdept_proj\c780_carel_cloud_engine_binary\Test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V.0.01" sheetId="3" r:id="rId1"/>
-    <sheet name="Instruction_Legenda" sheetId="5" r:id="rId2"/>
-    <sheet name="Support" sheetId="4" r:id="rId3"/>
+    <sheet name="initialization" sheetId="12" r:id="rId2"/>
+    <sheet name="wifi configuration" sheetId="6" r:id="rId3"/>
+    <sheet name="mqtt communication" sheetId="7" r:id="rId4"/>
+    <sheet name="modbus communication" sheetId="8" r:id="rId5"/>
+    <sheet name="CBOR encoding" sheetId="10" r:id="rId6"/>
+    <sheet name="default config" sheetId="9" r:id="rId7"/>
+    <sheet name="gsm configuration" sheetId="11" r:id="rId8"/>
+    <sheet name="Instruction_Legenda" sheetId="5" r:id="rId9"/>
+    <sheet name="Support" sheetId="4" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">V.0.01!$A$1:$F$361</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'V.0.01'!$A$1:$F$361</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +41,7 @@
     <author>Alessandro Bilato</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -58,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +84,476 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">if something was wrong a brief explanation of what happened
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alessandro Bilato</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Brief description of the scope of the test
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Test preconditions
+ie. Status of the connection, status of the monitored device etc.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Expected Result
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">if something was wrong a brief explanation of what happened
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alessandro Bilato</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Brief description of the scope of the test
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Test preconditions
+ie. Status of the connection, status of the monitored device etc.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Expected Result
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">if something was wrong a brief explanation of what happened
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alessandro Bilato</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Brief description of the scope of the test
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Test preconditions
+ie. Status of the connection, status of the monitored device etc.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Expected Result
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">if something was wrong a brief explanation of what happened
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alessandro Bilato</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Brief description of the scope of the test
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Test preconditions
+ie. Status of the connection, status of the monitored device etc.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Expected Result
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">if something was wrong a brief explanation of what happened
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alessandro Bilato</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Brief description of the scope of the test
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Test preconditions
+ie. Status of the connection, status of the monitored device etc.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Expected Result
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">if something was wrong a brief explanation of what happened
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alessandro Bilato</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Brief description of the scope of the test
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Test preconditions
+ie. Status of the connection, status of the monitored device etc.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Expected Result
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">if something was wrong a brief explanation of what happened
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alessandro Bilato</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Brief description of the scope of the test
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Test preconditions
+ie. Status of the connection, status of the monitored device etc.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Expected Result
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="164">
   <si>
     <t>Test ID</t>
   </si>
@@ -847,6 +1328,187 @@
   <si>
     <t>1. A Windows PC with a WiFi adapter/or a Smartphone 
 2. device with AP mode in default condition</t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed headers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor file whose header is badly formed </t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_set_gw_config paylaod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_set_gw_config file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_set_line_config paylaod</t>
+  </si>
+  <si>
+    <t>When GME receives the message, it detects the badly formed payload, discards it and goes back to reception</t>
+  </si>
+  <si>
+    <t>When GME receives the message, it detects the badly formed header, discards it and goes back to reception</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_set_line_config file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_set_devs_config paylaod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_set_devs_config file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_scan_devices paylaod</t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_read_values paylaod</t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_write_values paylaod</t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_change_cred paylaod</t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_gw_update paylaod</t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_dev_update paylaod</t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_reboot paylaod</t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_start_engine paylaod</t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_stop_engine paylaod</t>
+  </si>
+  <si>
+    <t>Check robustness with respect to malformed req_update_ca paylaod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_stop_engine file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_update_ca file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_start_engine file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_reboot file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_dev_update file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_gw_update file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_change_cred file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_write_values file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_read_values file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A cbor req_scan_devices file whose payload is badly formed </t>
+  </si>
+  <si>
+    <t>Tests from 1 to 14 aim at finding possible sw hunging 
+when receiving badly formatted payloads. If a payload is syntactically correct but fields have data type different from expected, GME may have unpredictable behavior.</t>
+  </si>
+  <si>
+    <t>Check connected payload</t>
+  </si>
+  <si>
+    <t>Check hello payload</t>
+  </si>
+  <si>
+    <t>Check status payload (only wifi)</t>
+  </si>
+  <si>
+    <t>Check mobile payload (only gsm)</t>
+  </si>
+  <si>
+    <t>Check alarms payload</t>
+  </si>
+  <si>
+    <t>Check values payload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with MqttClientSimulatorBinary installed </t>
+  </si>
+  <si>
+    <t>When GME sends a connected payload, it must contain 
+all required fields, e.g. 
+Connected: {“ver”:”100”, “ts”: 1574113297, “status”: 1}
+Check ts is correct time.</t>
+  </si>
+  <si>
+    <t>When GME sends a hello payload, it must contain 
+all required fields. Check fields content according to RS.</t>
+  </si>
+  <si>
+    <t>When GME sends a status payload, it must contain 
+all required fields. Check fields content according to RS. Check it is sent every pst seconds.</t>
+  </si>
+  <si>
+    <t>When GME sends a mobile payload, it must contain 
+all required fields. Check fields content according to RS. Check it is sent every 5 minutes.</t>
+  </si>
+  <si>
+    <t>1. A Windows PC with MqttClientSimulatorBinary installed 
+2. A c.pCO family controller connected</t>
+  </si>
+  <si>
+    <t>Force an alarm, check alarm payload is received and check fields content according to RS.
+Remove the alarm, check again alarm payload is received with proper fields in it.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check values payload is received and check fields content according to RS.  </t>
+  </si>
+  <si>
+    <t>This test does not aim at tyesting everything about values payload but just that syntax is correct.</t>
+  </si>
+  <si>
+    <t>Check that after default configuration is triggered, 
+GME actually starts with default configuration</t>
+  </si>
+  <si>
+    <t>Check default configuration is triggered 
+by pressing button with specific procedure</t>
+  </si>
+  <si>
+    <t>1. GME regularly running</t>
+  </si>
+  <si>
+    <t>NECESSARIO CAPIRE SE PUO' ESSERE FATTO PARTIRE IN OGNI MOMENTO O SOLO AL BOOT, DA VALUTARE INSIEME AL SECURE BOOT</t>
+  </si>
+  <si>
+    <t>RTC initialization</t>
+  </si>
+  <si>
+    <t>todo</t>
   </si>
 </sst>
 </file>
@@ -1048,11 +1710,186 @@
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="35">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1087,13 +1924,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
@@ -1108,14 +1938,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1123,20 +1946,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1415,7 +2224,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1425,9 +2234,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1473,9 +2282,6 @@
       <c r="D2" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="3" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="25">
@@ -1979,18 +2785,18 @@
   </sheetData>
   <autoFilter ref="A1:F361"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="34" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="33" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="31" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2027,7 +2833,2941 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="31" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
+        <f t="shared" ref="A5:A33" si="0">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="25">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="25">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="25">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="25">
+        <v>33</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E35" s="18"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Support!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E362</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="31" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
+        <f t="shared" ref="A5:A33" si="0">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="25">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="25">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="25">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="25">
+        <v>33</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E35" s="18"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Support!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E362</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="31" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
+        <f t="shared" ref="A5:A33" si="0">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="25">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="25">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="25">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="25">
+        <v>33</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E35" s="18"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Support!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E362</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="31" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
+        <f t="shared" ref="A5:A33" si="0">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="25">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="25">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="25">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="25">
+        <v>33</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E35" s="18"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Support!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E362</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
+        <f t="shared" ref="A5:A33" si="0">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13" s="15"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="15"/>
+      <c r="F21" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="25">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="25">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="25">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="25">
+        <v>33</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E35" s="18"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Support!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E362</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C22:C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="31" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
+        <f t="shared" ref="A5:A33" si="0">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="25">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="25">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="25">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="25">
+        <v>33</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E35" s="18"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Support!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E362</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="31" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
+        <f t="shared" ref="A5:A33" si="0">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="15"/>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="16"/>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="15"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="25">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="21"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="25">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="25">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="30"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="25">
+        <v>33</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E35" s="18"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Support!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E362</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
@@ -2099,40 +5839,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
test plan: doc updated with some test cases
</commit_message>
<xml_diff>
--- a/Test/C780_Binary_Library_Test_Plan.xlsx
+++ b/Test/C780_Binary_Library_Test_Plan.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="V.0.01" sheetId="3" r:id="rId1"/>
-    <sheet name="initialization" sheetId="12" r:id="rId2"/>
+    <sheet name="rtc configuration" sheetId="12" r:id="rId2"/>
     <sheet name="wifi configuration" sheetId="6" r:id="rId3"/>
     <sheet name="mqtt communication" sheetId="7" r:id="rId4"/>
     <sheet name="modbus communication" sheetId="8" r:id="rId5"/>
@@ -24,7 +24,7 @@
     <sheet name="Support" sheetId="4" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'V.0.01'!$A$1:$F$361</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'V.0.01'!$A$1:$F$357</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="172">
   <si>
     <t>Test ID</t>
   </si>
@@ -621,27 +621,9 @@
 of start up</t>
   </si>
   <si>
-    <t xml:space="preserve">1. A Windows PC with a WiFi adapter
-2. device with AP mode in default condition
-3. Use the PC and connect to the SSID "GME_ xxyyzz" </t>
-  </si>
-  <si>
-    <t>1. the PC is able to connect to the AP
-2. the AP don't ask for a password
-3. the DHCP of the device assign the address 192.168.100.10 
-    to  the PC 
-4. the default gateway returned is 192.168.100.1
-Note. Use command line console with the "ipconfig /all" command
-to verify the above data.</t>
-  </si>
-  <si>
     <t>1. A Windows PC with a WiFi connected to the AP</t>
   </si>
   <si>
-    <t>1. open a browser and type "http://192.168.100.1"
-2. the broweser show the device configuration page</t>
-  </si>
-  <si>
     <t xml:space="preserve">Test that device AP emit the right SSID </t>
   </si>
   <si>
@@ -651,9 +633,6 @@
     <t>Test that the device webserver respond</t>
   </si>
   <si>
-    <t>Test that the device is able to connect to an AP</t>
-  </si>
-  <si>
     <t>Device AP</t>
   </si>
   <si>
@@ -670,18 +649,6 @@
   </si>
   <si>
     <t>Note</t>
-  </si>
-  <si>
-    <t>1. A Windows PC with a WiFi connected to the AP
-2. browser pointing to "http://192.168.100.1"
-3. set the parameters as follow
-   - AP SSID "TEST_AP" 
-   - AP Security : WPA
-   - AP Password : "12345678"
-   - DHCP on</t>
-  </si>
-  <si>
-    <t>1. the configuration page is able to receive the configuration parameters</t>
   </si>
   <si>
     <t>Instructions</t>
@@ -695,31 +662,6 @@
     <t>Test the device webserver configuration page</t>
   </si>
   <si>
-    <t>1. a test AP connected to the internet 
-     configured as follow :
-   - SSID "TEST_AP" 
-   - Security : WPA
-   - Password : "12345678"
-   - DHCP on
-   - DHCP base address 192.168.0.100
-   - AP address 192.168.0.1 
-   - DNS 8.8.8.8/8.8.4.4
-2. a device with all the connections parameter already configured as above</t>
-  </si>
-  <si>
-    <t>1. the device is able to connect to the AP
-2. through the debug console of the device, check that
-    a. the IP address is 192.168.0.100
-    b. the default gateway is 192.168.0.1
-    c. the DNS is 8.8.8.8/8.8.4.4</t>
-  </si>
-  <si>
-    <t>1. the device is powered off
-2. a test AP configured as previous test 
-3. the default NTP server must be reachable, check it with a PC.
-4. power on the device</t>
-  </si>
-  <si>
     <t>Check with the debug console that the INT32 var that contain the UTC value, the number must be comparable with the current time returned by https://www.epochconverter.com/</t>
   </si>
   <si>
@@ -728,17 +670,8 @@
 3. power on the device</t>
   </si>
   <si>
-    <t>Check with the debug console that the INT32 var that contain the UTC value, the converted value is within 1970/01/01 range use 
-https://www.epochconverter.com/</t>
-  </si>
-  <si>
     <t>Test if the device configuration is maintained 
 between power on/off cycle.</t>
-  </si>
-  <si>
-    <t>1. if the previous test is ok, power off the device
-and wait 5 seconds.
-2. power on again the device</t>
   </si>
   <si>
     <t>1. the device is able to connect to the AP
@@ -749,9 +682,6 @@
 3. open a browser and type "http://192.168.100.1"
     the device configuration page contains the values set in the
     previous test.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> payload-alarms.json</t>
   </si>
   <si>
     <t xml:space="preserve"> payload-change_credentials-req.json</t>
@@ -1300,17 +1230,6 @@
     from 1 &gt; 0 </t>
   </si>
   <si>
-    <t>1. the system respond with a JSON packet with the alarm 
-payload (A) like .\Documents\specs\payload-alarms.json
-2. copy and paste the payload into the validation tool https://jsonformatter.curiousconcept.com/ and verify it
-3. verify if the "startime" value is the current time
-    "endtime" must be equal to 0
-4. wait the alarm close payload (B)
-5. copy and paste the payload into the validation tool https://jsonformatter.curiousconcept.com/ and verify it
-3. verify if the "startime" value is the same as point 3
-    "endtime" must be equal to the current time</t>
-  </si>
-  <si>
     <t>1. the cpCO connected to the gateway
 2. Send a request from the cloud to the target
 use the example in the test directory  test-send_mb_adu-req.json</t>
@@ -1322,14 +1241,6 @@
 it contains the raw data response to the command</t>
   </si>
   <si>
-    <t>Use the PC/Smartphone to discover the SSID, you will find an SSID like
-"GME_ xxyyzz" where xxyyzz are tha last MAC address numbers of the device</t>
-  </si>
-  <si>
-    <t>1. A Windows PC with a WiFi adapter/or a Smartphone 
-2. device with AP mode in default condition</t>
-  </si>
-  <si>
     <t>Check robustness with respect to malformed headers</t>
   </si>
   <si>
@@ -1505,10 +1416,143 @@
     <t>NECESSARIO CAPIRE SE PUO' ESSERE FATTO PARTIRE IN OGNI MOMENTO O SOLO AL BOOT, DA VALUTARE INSIEME AL SECURE BOOT</t>
   </si>
   <si>
-    <t>RTC initialization</t>
-  </si>
-  <si>
-    <t>todo</t>
+    <t>1. the device is powered off
+2. a test AP configured 
+3. the default NTP server must be reachable, check it with a PC.
+4. power on the device</t>
+  </si>
+  <si>
+    <t>Check with the debug console that the INT32 var that contain the UTC value, the converted value is within 1970/01/01 range use 
+https://www.epochconverter.com/
+GME must not reboot, it must be possible to reconfigure the ntp server using the web page</t>
+  </si>
+  <si>
+    <t>1. the PC is able to connect to the AP
+2. the AP doesn't ask for a password
+3. the DHCP of the device assign the address 10.10.100.10 
+    to  the PC 
+4. the default gateway returned is 10.10.100.254
+Note. Use command line console with the "ipconfig /all" command
+to verify the above data.</t>
+  </si>
+  <si>
+    <t>Use the PC/Smartphone to discover the SSID, you will find an SSID like
+"cgatem_ xxyyzz" where xxyyzz are tha last MAC address numbers of the device</t>
+  </si>
+  <si>
+    <t>Test the device webserver login page</t>
+  </si>
+  <si>
+    <t>1. open a browser and type "http://10.10.100.10"
+2. the broweser shows the device login page</t>
+  </si>
+  <si>
+    <t>1. A Windows PC with a WiFi connected to the AP
+2. browser pointing to "http://10.10.100.10". set the parameters as follow
+   - AP SSID "TEST_AP" 
+   - AP Security : WPA
+   - AP Password : "12345678"
+   - DHCP on</t>
+  </si>
+  <si>
+    <t>1. the device is able to connect to the AP
+2. through the debug console of the device, check that
+    a. the IP address is 10.10.100.10
+    b. the default gateway is 10.10.100.254
+    c. the DNS is 8.8.8.8/8.8.4.4</t>
+  </si>
+  <si>
+    <t>1. the login page is able to receive the login information
+2. When submit is clicked, the config page appears</t>
+  </si>
+  <si>
+    <t>1. A Windows PC with a WiFi adapter. Repeat all the below tests using a a smartphone.
+2. device with AP mode in default condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A Windows PC with a WiFi adapter (smartphone)
+2. device with AP mode in default condition
+3. Use the PC and connect to the SSID "cgatem_ xxyyzz" </t>
+  </si>
+  <si>
+    <t>1. a test AP connected to the internet 
+     configured as follow :
+   - SSID "TEST_AP" 
+   - Security : WPA
+   - Password : "12345678"
+   - DHCP on
+2. a device with all the connections parameter already configured as above</t>
+  </si>
+  <si>
+    <t>1. the configuration page is able to receive the configuration parameters (check at GME reboot)</t>
+  </si>
+  <si>
+    <t>Test that the device is able to connect to an AP
+ manually selected</t>
+  </si>
+  <si>
+    <t>Test that the device is able to connect to an AP
+  selected with a wifi scan</t>
+  </si>
+  <si>
+    <t>Test that the device is able to connect to an AP
+ configured with WPS</t>
+  </si>
+  <si>
+    <t>1. a test AP connected to the internet 
+     configured as follow :
+   - SSID "TEST_AP" 
+   - Security : WPA
+   - Password : "12345678"
+   - DHCP on
+2. a device with all the connections parameter already configured as above
+3. select the desired wifi AP from the list menu</t>
+  </si>
+  <si>
+    <t>1. a test AP connected to the internet 
+     configured as follow :
+   - SSID "TEST_AP" 
+   - Security : WPA
+   - Password : "12345678"
+   - DHCP on
+2. a device with all the connections parameter already configured as above
+3. select the WPS choice and then press the WPS button on the AP (according to your AP manual)</t>
+  </si>
+  <si>
+    <t>1. if the previous tests are ok, power off the device
+and wait 5 seconds.
+2. power on again the device</t>
+  </si>
+  <si>
+    <t>Test that the device is able to connect to an AP
+ with static IP configuration</t>
+  </si>
+  <si>
+    <t>1. a test AP connected to the internet 
+     configured as follow :
+   - SSID "TEST_AP" 
+   - Security : WPA
+   - Password : "12345678"
+2. a device with all the connections parameter already configured as above
+3. select DHCP off
+4. fill the textboxes with IP address and other static configuration info</t>
+  </si>
+  <si>
+    <t>1. the device is able to connect to the AP
+2. through the debug D17console of the device, check that the IP address, the default gateway and the DNS are the ones configured</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> payload-alarms.cbor</t>
+  </si>
+  <si>
+    <t>All below tests require that GME is connected to an AP and that a MQTT server is reachable. 
+It also requires that a c.pCO is properly connected to the serial port of the GME, that configuration is completed and GME has a valid model on board. Use a proper application for c.pCO showing some alarm variables, and a reasonable number of HR, IR, DI and COIL.
+Use MQTTClientSimulatorBinary in http://svncarel.carel.com/svn/c780_carel_cloud_engine_binary/Utility/MqttClientSimulatorBinary/MqttClientSimulatorBinary
+This works as a sniffer and shows the decoded CBOR stream</t>
+  </si>
+  <si>
+    <t>Check that when the alarm is triggered a message is logged with st field containing the timestamp related to the beginning of the alarm, et 0. 
+When the alarm reenters another alarm message is sent with st as the first message and et current time. Check all other fileds according to specification.</t>
   </si>
 </sst>
 </file>
@@ -1710,7 +1754,7 @@
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="50">
     <dxf>
       <fill>
         <patternFill>
@@ -1826,7 +1870,98 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1889,7 +2024,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1903,21 +2038,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1945,6 +2066,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -1952,7 +2080,28 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2232,11 +2381,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2269,204 +2418,212 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="144" x14ac:dyDescent="0.3">
       <c r="A2" s="25">
         <v>1</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="25">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A23" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
-        <f>A3+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="25">
-        <f t="shared" ref="A5:A33" si="0">A4+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="C5" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="25">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+    </row>
+    <row r="7" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="25">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="6" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="25">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="28" t="s">
+      <c r="C8" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="15"/>
+    </row>
+    <row r="9" spans="1:6" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="15"/>
+    </row>
+    <row r="11" spans="1:6" s="8" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="25">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="25">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="25">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="19" t="s">
+      <c r="C13" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D10" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="144" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="25">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="1:6" s="8" customFormat="1" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="25">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>60</v>
+      <c r="B14" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="E14" s="15"/>
     </row>
@@ -2476,348 +2633,207 @@
         <v>14</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" s="10" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="25">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <v>33</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="26"/>
+      <c r="B25" s="31"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="26"/>
+      <c r="B26" s="31"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26" s="13"/>
+    </row>
+    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F28" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="8" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="1:6" s="8" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="25">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="1:6" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:6" s="8" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="25">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="1:6" s="8" customFormat="1" ht="144" x14ac:dyDescent="0.3">
-      <c r="A21" s="25">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="1:6" s="10" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="25">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="1:6" s="8" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A23" s="25">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" spans="1:6" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="25">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" spans="1:6" s="8" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="25">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="15"/>
-    </row>
-    <row r="26" spans="1:6" s="8" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="25">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="8" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="25">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>102</v>
-      </c>
-      <c r="E27" s="15"/>
-    </row>
-    <row r="28" spans="1:6" s="8" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A28" s="25">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="E28" s="15"/>
-    </row>
-    <row r="29" spans="1:6" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="25">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="21" t="s">
+    </row>
+    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F29" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="30" spans="1:6" s="8" customFormat="1" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A30" s="25">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="15"/>
-    </row>
-    <row r="31" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="25">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="25">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="F32" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="25">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="F33" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="25">
-        <v>33</v>
-      </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E35" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F361"/>
+  <autoFilter ref="A1:F357"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="34" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="39" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="38" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="2" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="BLOCKING">
-      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="31" priority="3" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="containsText" dxfId="37" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C20" r:id="rId1" display="Test_cases\JSON_test_cases\test-set_devs_config-req.json"/>
-    <hyperlink ref="C18" r:id="rId2" display="Test_cases\JSON_test_cases\test-scan_line-req.json"/>
-    <hyperlink ref="C17" r:id="rId3" display="Test_cases\JSON_test_cases\test-read_values-req.json"/>
-    <hyperlink ref="C14" r:id="rId4" display="Test_cases\JSON_test_cases\test-change_credentials-req.json"/>
-    <hyperlink ref="C22" r:id="rId5" display="Test_cases\JSON_test_cases\test-set_lines_config-req.json"/>
-    <hyperlink ref="C25" r:id="rId6" display="Test_cases\JSON_test_cases\test-update_ca_cerficates-req.json"/>
-    <hyperlink ref="C26" r:id="rId7" display="Test_cases\JSON_test_cases\test-update_dev_firmware-req.json"/>
-    <hyperlink ref="C27" r:id="rId8" display="Test_cases\JSON_test_cases\test-update_gw_firmware-req.json"/>
-    <hyperlink ref="C21" r:id="rId9" display="Test_cases\JSON_test_cases\test-set_devs_config-req.json"/>
-    <hyperlink ref="D15" r:id="rId10" display="..\Documents\specs\payload-hello.json"/>
-    <hyperlink ref="D23" r:id="rId11" display="..\Documents\specs\payload-status.json"/>
-    <hyperlink ref="D13" r:id="rId12" display="..\Documents\specs\payload-alarms.json"/>
-    <hyperlink ref="C19" r:id="rId13" display="Test_cases\JSON_test_cases\test-send_mb_adu-req.json"/>
+    <hyperlink ref="C10" r:id="rId1" display="Test_cases\JSON_test_cases\test-set_devs_config-req.json"/>
+    <hyperlink ref="C8" r:id="rId2" display="Test_cases\JSON_test_cases\test-scan_line-req.json"/>
+    <hyperlink ref="C7" r:id="rId3" display="Test_cases\JSON_test_cases\test-read_values-req.json"/>
+    <hyperlink ref="C4" r:id="rId4" display="Test_cases\JSON_test_cases\test-change_credentials-req.json"/>
+    <hyperlink ref="C12" r:id="rId5" display="Test_cases\JSON_test_cases\test-set_lines_config-req.json"/>
+    <hyperlink ref="C15" r:id="rId6" display="Test_cases\JSON_test_cases\test-update_ca_cerficates-req.json"/>
+    <hyperlink ref="C16" r:id="rId7" display="Test_cases\JSON_test_cases\test-update_dev_firmware-req.json"/>
+    <hyperlink ref="C17" r:id="rId8" display="Test_cases\JSON_test_cases\test-update_gw_firmware-req.json"/>
+    <hyperlink ref="C11" r:id="rId9" display="Test_cases\JSON_test_cases\test-set_devs_config-req.json"/>
+    <hyperlink ref="D5" r:id="rId10" display="..\Documents\specs\payload-hello.json"/>
+    <hyperlink ref="D13" r:id="rId11" display="..\Documents\specs\payload-status.json"/>
+    <hyperlink ref="C9" r:id="rId12" display="Test_cases\JSON_test_cases\test-send_mb_adu-req.json"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
-  <legacyDrawing r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <legacyDrawing r:id="rId14"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -2825,7 +2841,7 @@
           <x14:formula1>
             <xm:f>Support!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E362</xm:sqref>
+          <xm:sqref>E2:E352</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2871,10 +2887,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2907,31 +2923,949 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="25">
         <v>1</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>162</v>
+        <v>10</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <f t="shared" ref="A3:A4" si="0">A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
+        <f t="shared" ref="A5:A32" si="1">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="25">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="15"/>
+    </row>
+    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="16"/>
+    </row>
+    <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="28"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="15"/>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="21"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="25">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="25">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="25">
+        <v>33</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="18"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1 E5:E1048576">
+    <cfRule type="containsText" dxfId="36" priority="4" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="5" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="7" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="containsText" dxfId="33" priority="6" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E4">
+    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="3" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Support!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E361</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="31" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="25">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="B3" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
+        <v>4</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
+        <f>A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="25">
+        <f t="shared" ref="A7:A9" si="0">A6+1</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
+        <v>9</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>166</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <f>A10+1</f>
+        <v>10</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <f t="shared" ref="A12:A37" si="1">A11+1</f>
+        <v>11</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+    </row>
+    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="25">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="25">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="15"/>
+    </row>
+    <row r="26" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="15"/>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="15"/>
+    </row>
+    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="25">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="15"/>
+    </row>
+    <row r="32" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="25">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="27"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="15"/>
+    </row>
+    <row r="33" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="25">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="27"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="25">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="27"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="15"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="25">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="28"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="21"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="25">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="30"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="25">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="30"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="25">
+        <v>33</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E39" s="18"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1 E12:E1048576">
+    <cfRule type="containsText" dxfId="29" priority="4" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="5" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="containsText" dxfId="26" priority="6" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F6)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E11">
+    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Support!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E366</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="31" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
+        <v>0</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
         <f>A3+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="27"/>
       <c r="C4" s="19"/>
@@ -2940,7 +3874,7 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="25">
         <f t="shared" ref="A5:A33" si="0">A4+1</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="27"/>
       <c r="C5" s="19"/>
@@ -2949,7 +3883,7 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="25">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="27"/>
       <c r="C6" s="19"/>
@@ -2958,7 +3892,7 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="25">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="19"/>
@@ -2967,7 +3901,7 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="25">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="19"/>
@@ -2976,7 +3910,7 @@
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="25">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="27"/>
       <c r="C9" s="19"/>
@@ -2985,7 +3919,7 @@
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="25">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="19"/>
@@ -2994,7 +3928,7 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="25">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="27"/>
       <c r="C11" s="19"/>
@@ -3003,7 +3937,7 @@
     <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="25">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="27"/>
       <c r="C12" s="21"/>
@@ -3013,7 +3947,7 @@
     <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="25">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="27"/>
       <c r="C13" s="21"/>
@@ -3024,7 +3958,7 @@
     <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="25">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="27"/>
       <c r="C14" s="22"/>
@@ -3034,7 +3968,7 @@
     <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="25">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="27"/>
       <c r="C15" s="21"/>
@@ -3044,7 +3978,7 @@
     <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="25">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="27"/>
       <c r="C16" s="15"/>
@@ -3055,7 +3989,7 @@
     <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="25">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="27"/>
       <c r="C17" s="22"/>
@@ -3065,7 +3999,7 @@
     <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="25">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="27"/>
       <c r="C18" s="22"/>
@@ -3075,7 +4009,7 @@
     <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="25">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="29"/>
       <c r="C19" s="22"/>
@@ -3085,7 +4019,7 @@
     <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="25">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="22"/>
@@ -3095,7 +4029,7 @@
     <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="25">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="27"/>
       <c r="C21" s="22"/>
@@ -3105,7 +4039,7 @@
     <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="29"/>
       <c r="C22" s="22"/>
@@ -3115,7 +4049,7 @@
     <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="25">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" s="27"/>
       <c r="C23" s="23"/>
@@ -3125,7 +4059,7 @@
     <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="25">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" s="28"/>
       <c r="C24" s="23"/>
@@ -3135,7 +4069,7 @@
     <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="25">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="22"/>
@@ -3145,7 +4079,7 @@
     <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="25">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="22"/>
@@ -3156,7 +4090,7 @@
     <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="25">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="27"/>
       <c r="C27" s="22"/>
@@ -3166,7 +4100,7 @@
     <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="25">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="27"/>
       <c r="C28" s="19"/>
@@ -3176,7 +4110,7 @@
     <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="25">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="27"/>
       <c r="C29" s="19"/>
@@ -3186,7 +4120,7 @@
     <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="25">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="27"/>
       <c r="C30" s="19"/>
@@ -3196,7 +4130,7 @@
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="25">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="28"/>
       <c r="C31" s="19"/>
@@ -3205,7 +4139,7 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="25">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="30"/>
       <c r="C32" s="13"/>
@@ -3215,7 +4149,7 @@
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="25">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="30"/>
       <c r="C33" s="13"/>
@@ -3234,20 +4168,31 @@
       <c r="E35" s="18"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="23" priority="1" operator="containsText" text="BLOCKING">
+  <conditionalFormatting sqref="E1:E2 E4:E1048576">
+    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="20" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="19" priority="6" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3267,406 +4212,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40" style="31" customWidth="1"/>
-    <col min="3" max="3" width="67.33203125" customWidth="1"/>
-    <col min="4" max="4" width="56" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="25">
-        <v>1</v>
-      </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="25">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="25">
-        <f>A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="25">
-        <f t="shared" ref="A5:A33" si="0">A4+1</f>
-        <v>4</v>
-      </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="25">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="25">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="25">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="25">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="25">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-    </row>
-    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="25">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="25">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="25">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="25">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="25">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="25">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="25">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="15"/>
-    </row>
-    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="25">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="25">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="15"/>
-    </row>
-    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="25">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="15"/>
-    </row>
-    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="25">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="25">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="15"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="25">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="21"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="25">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="F32" s="11"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="25">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="F33" s="11"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="25">
-        <v>33</v>
-      </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E35" s="18"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="BLOCKING">
-      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Support!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E362</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4055,18 +4606,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40" style="31" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67.33203125" customWidth="1"/>
     <col min="4" max="4" width="56" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
@@ -4093,196 +4644,322 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="25">
         <v>1</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="25">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="25">
         <f t="shared" ref="A5:A33" si="0">A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="25">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="25">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="28"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="25">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="25">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="25">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="25">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-    </row>
-    <row r="12" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="25">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
+      <c r="B12" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="25">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="22"/>
+      <c r="B13" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="E13" s="15"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="25">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="21"/>
+      <c r="B14" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="25">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="22"/>
+      <c r="B15" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="25">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
+      <c r="B16" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>135</v>
+      </c>
       <c r="E16" s="15"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="25">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="21"/>
+      <c r="B17" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>136</v>
+      </c>
       <c r="E17" s="15"/>
     </row>
-    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="25">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="21"/>
+      <c r="B18" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>137</v>
+      </c>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="25">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="21"/>
+      <c r="B19" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>138</v>
+      </c>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="25">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="21"/>
+      <c r="B20" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>140</v>
+      </c>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="25">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="21"/>
+      <c r="B21" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>141</v>
+      </c>
       <c r="E21" s="15"/>
+      <c r="F21" s="8" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="25">
@@ -4449,532 +5126,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.33203125" customWidth="1"/>
-    <col min="4" max="4" width="56" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="25">
-        <v>1</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>112</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="25">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="25">
-        <f>A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="25">
-        <f t="shared" ref="A5:A33" si="0">A4+1</f>
-        <v>4</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="25">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="D6" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="25">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="25">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="25">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="25">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="25">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="E12" s="15"/>
-    </row>
-    <row r="13" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="25">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14" s="15"/>
-    </row>
-    <row r="15" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="E15" s="15"/>
-    </row>
-    <row r="16" spans="1:6" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="25">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="12"/>
-    </row>
-    <row r="17" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>151</v>
-      </c>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="1:6" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="25">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>145</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>152</v>
-      </c>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="1:6" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="25">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:6" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="25">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="1:6" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="25">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="E21" s="15"/>
-      <c r="F21" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="25">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="25">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="15"/>
-    </row>
-    <row r="24" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="25">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="15"/>
-    </row>
-    <row r="25" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="25">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="15"/>
-    </row>
-    <row r="26" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="25">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="12"/>
-    </row>
-    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="25">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="15"/>
-    </row>
-    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="25">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="15"/>
-    </row>
-    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="25">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="15"/>
-    </row>
-    <row r="30" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="25">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="15"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="25">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="21"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="25">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="F32" s="11"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="25">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="F33" s="11"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="25">
-        <v>33</v>
-      </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E35" s="18"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="BLOCKING">
-      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="4" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Support!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E362</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C22:C23"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5012,13 +5169,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -5027,10 +5184,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D3" s="19"/>
     </row>
@@ -5341,18 +5498,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5735,18 +5892,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5784,34 +5941,34 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -5833,7 +5990,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test plan: doc updated with some test cases (modbus)
</commit_message>
<xml_diff>
--- a/Test/C780_Binary_Library_Test_Plan.xlsx
+++ b/Test/C780_Binary_Library_Test_Plan.xlsx
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="204">
   <si>
     <t>Test ID</t>
   </si>
@@ -615,10 +615,6 @@
   <si>
     <t>The system is running and correctly synchronized 
 with the NTP server</t>
-  </si>
-  <si>
-    <t>Inspect the variable Power_On_Time and this report the UTC time
-of start up</t>
   </si>
   <si>
     <t>1. A Windows PC with a WiFi connected to the AP</t>
@@ -685,9 +681,6 @@
   <si>
     <t>Si usa il cpCO ono 2 file di modello con diffreneti 
 isteresi  a parità di parametro</t>
-  </si>
-  <si>
-    <t>This test will be possible only after the new cpCO OS with Modbus file transfer will be available, end on July 2019</t>
   </si>
   <si>
     <t>Si usa il cpCO ono 2 file di modello con diffreneti 
@@ -1365,6 +1358,94 @@
   </si>
   <si>
     <t>payload_mobile</t>
+  </si>
+  <si>
+    <t>parity</t>
+  </si>
+  <si>
+    <t>stop bit</t>
+  </si>
+  <si>
+    <t>baud rate</t>
+  </si>
+  <si>
+    <t>model check (comprendendo anche il caso: "cosa succede se il modello è sbagliato per qualche ragione?")</t>
+  </si>
+  <si>
+    <t>fragmentation</t>
+  </si>
+  <si>
+    <t>Inspect the variable Power_On_Time in hello packet and this report the UTC time of start up</t>
+  </si>
+  <si>
+    <t>a. Set baud rate to 9600 bps with a properly formed CBOR payload set_lines_config
+b. Set baud rate to 19200 bps with proper payload</t>
+  </si>
+  <si>
+    <t>connettore RS485</t>
+  </si>
+  <si>
+    <t>Set connector type RS485 with set_lines_config</t>
+  </si>
+  <si>
+    <t>connettore ttl</t>
+  </si>
+  <si>
+    <t>Set connector type ttl with set_lines_config</t>
+  </si>
+  <si>
+    <t>Check that something is coming out from ttl serial 
+using an oscilloscope</t>
+  </si>
+  <si>
+    <t>In both cases, baud rate of the serial must change to the chosen values. Check with an oscilloscope or connecting a device having the required serial speed</t>
+  </si>
+  <si>
+    <t>Check that something is coming out from RS485 serial 
+using an oscilloscope (for this to happen GME must have been previously configured, the same applies for successive tests)</t>
+  </si>
+  <si>
+    <t>Check with an oscilloscope</t>
+  </si>
+  <si>
+    <t>a. Set parity to even 
+b. Set parity to odd
+c. Set parity to none</t>
+  </si>
+  <si>
+    <t>a. Set stop bit to 1
+b. Set stop bit to 2</t>
+  </si>
+  <si>
+    <t>repeat configuration tests for ttl connector 
+(from #2 to #4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check with an oscilloscope.
+Verify that with polling delay 0 gme polls without delays between a packet and the following
+Verify that with polling delay 200 gme polls with 200ms delay between a packet and the following
+</t>
+  </si>
+  <si>
+    <t>a. Set polling delay to 0
+b. Set polling delay to 200ms</t>
+  </si>
+  <si>
+    <t>linearization</t>
+  </si>
+  <si>
+    <t>hysteresis</t>
+  </si>
+  <si>
+    <t>Use an application with 2 parameters having different linearization values. 
+Change the 2 values</t>
+  </si>
+  <si>
+    <t>Verify that linearization is properly applied to both variables</t>
+  </si>
+  <si>
+    <t>Use an application with 2 parameters having different hysteresis values. 
+Change the 2 values</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1559,6 +1640,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2127,7 +2211,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2160,20 +2244,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="e">
         <f>#REF!+1</f>
         <v>#REF!</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="10" t="s">
-        <v>35</v>
-      </c>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="e">
@@ -2181,7 +2263,7 @@
         <v>#REF!</v>
       </c>
       <c r="B3" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -2212,12 +2294,12 @@
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F8" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F9" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2292,7 +2374,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2333,10 +2415,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -2348,10 +2430,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2366,7 +2448,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>14</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -2405,29 +2487,23 @@
       <c r="C8" s="16"/>
       <c r="D8" s="16"/>
     </row>
-    <row r="9" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="16"/>
-      <c r="D9" s="16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="21">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B10" s="23"/>
-      <c r="C10" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>150</v>
-      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
     </row>
     <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
@@ -2481,36 +2557,24 @@
       <c r="E15" s="12"/>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="B16" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>154</v>
-      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="B17" s="23" t="s">
-        <v>152</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>156</v>
-      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -2762,13 +2826,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -2777,13 +2841,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2792,13 +2856,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -2807,13 +2871,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>110</v>
-      </c>
       <c r="D5" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2822,13 +2886,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>92</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -2837,13 +2901,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -2852,13 +2916,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
@@ -2867,13 +2931,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>101</v>
-      </c>
       <c r="D9" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -2882,13 +2946,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -2896,13 +2960,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -2911,13 +2975,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -2926,13 +2990,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2941,13 +3005,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -2956,13 +3020,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>123</v>
-      </c>
       <c r="D15" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -2971,13 +3035,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>153</v>
-      </c>
       <c r="D16" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -2986,13 +3050,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E17" s="12"/>
     </row>
@@ -3269,8 +3333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3309,7 +3373,7 @@
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D2" s="16"/>
     </row>
@@ -3319,13 +3383,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>105</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>107</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -3335,13 +3399,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="16" t="s">
         <v>125</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -3350,13 +3414,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>128</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
@@ -3365,13 +3429,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
@@ -3380,13 +3444,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C7" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>134</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="72" x14ac:dyDescent="0.3">
@@ -3395,13 +3459,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>144</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
@@ -3410,13 +3474,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
@@ -3425,13 +3489,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
@@ -3440,13 +3504,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -3455,13 +3519,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -3470,13 +3534,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E13" s="12"/>
     </row>
@@ -3486,13 +3550,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="7"/>
@@ -3503,13 +3567,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C15" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>165</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>167</v>
       </c>
       <c r="E15" s="12"/>
     </row>
@@ -3519,13 +3583,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>153</v>
-      </c>
       <c r="D16" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E16" s="12"/>
     </row>
@@ -3535,13 +3599,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="10"/>
@@ -3552,13 +3616,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E18" s="12"/>
     </row>
@@ -3568,13 +3632,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C19" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>170</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>172</v>
       </c>
       <c r="E19" s="12"/>
     </row>
@@ -3584,13 +3648,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="C20" s="17" t="s">
-        <v>175</v>
-      </c>
       <c r="D20" s="17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E20" s="12"/>
     </row>
@@ -3600,13 +3664,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>176</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>178</v>
       </c>
       <c r="E21" s="12"/>
     </row>
@@ -3616,10 +3680,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="29" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="12"/>
@@ -3630,10 +3694,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="13"/>
@@ -3643,7 +3707,9 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="23"/>
+      <c r="B24" s="23" t="s">
+        <v>183</v>
+      </c>
       <c r="C24" s="19"/>
       <c r="D24" s="18"/>
       <c r="E24" s="12"/>
@@ -3807,10 +3873,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3843,177 +3909,213 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="21">
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>181</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="23" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
-        <f t="shared" ref="A5:A33" si="0">A4+1</f>
+        <f>A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f t="shared" si="0"/>
+        <f>A5+1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A7:A38" si="0">A6+1</f>
         <v>6</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="16"/>
+      <c r="B7" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="11"/>
       <c r="D7" s="16"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="21">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="21">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="21">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="16"/>
+      <c r="B8" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="21"/>
+      <c r="B9" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="21"/>
+      <c r="B10" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>203</v>
+      </c>
       <c r="D10" s="16"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="23"/>
+        <f>A8+1</f>
+        <v>8</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>175</v>
+      </c>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
     </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
         <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="21">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="21">
+      <c r="B14" s="23"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="21">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21">
+      <c r="B15" s="23"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="21">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
       <c r="B16" s="23"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="10"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="21">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" s="23"/>
-      <c r="C17" s="18"/>
+      <c r="C17" s="17"/>
       <c r="D17" s="17"/>
       <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="23"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
       <c r="E18" s="12"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="25"/>
+        <v>16</v>
+      </c>
+      <c r="B19" s="23"/>
       <c r="C19" s="18"/>
       <c r="D19" s="17"/>
       <c r="E19" s="12"/>
@@ -4021,57 +4123,58 @@
     <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="23"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="12"/>
     </row>
     <row r="21" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="23"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="17"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="12"/>
-    </row>
-    <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="25"/>
+        <v>19</v>
+      </c>
+      <c r="B22" s="23"/>
       <c r="C22" s="18"/>
       <c r="D22" s="17"/>
-      <c r="E22" s="13"/>
+      <c r="E22" s="12"/>
     </row>
     <row r="23" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" s="23"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
       <c r="E23" s="12"/>
     </row>
     <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21">
         <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="16"/>
+        <v>21</v>
+      </c>
+      <c r="B24" s="25"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="17"/>
       <c r="E24" s="12"/>
     </row>
     <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="18"/>
@@ -4081,93 +4184,143 @@
     <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="18"/>
       <c r="D26" s="17"/>
       <c r="E26" s="12"/>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B27" s="25"/>
       <c r="C27" s="18"/>
       <c r="D27" s="17"/>
-      <c r="E27" s="12"/>
+      <c r="E27" s="13"/>
     </row>
     <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" s="23"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="17"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="18"/>
       <c r="E28" s="12"/>
     </row>
     <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21">
         <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="B29" s="24"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="16"/>
       <c r="E29" s="12"/>
     </row>
     <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30" s="23"/>
-      <c r="C30" s="16"/>
+      <c r="C30" s="18"/>
       <c r="D30" s="17"/>
       <c r="E30" s="12"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21">
         <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="21">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B32" s="23"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="12"/>
+    </row>
+    <row r="33" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="21">
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="17"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="21">
+      <c r="B33" s="23"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="12"/>
+    </row>
+    <row r="34" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="21">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="21">
+      <c r="B34" s="23"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="12"/>
+    </row>
+    <row r="35" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="21">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="21">
+      <c r="B35" s="23"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="12"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="21">
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E35" s="15"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="21">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B37" s="26"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="F37" s="9"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="21">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B38" s="26"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="21">
+        <v>33</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E40" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
@@ -4181,13 +4334,14 @@
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
+  <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FAIL",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -4195,7 +4349,7 @@
           <x14:formula1>
             <xm:f>Support!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E362</xm:sqref>
+          <xm:sqref>E2:E367</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4207,7 +4361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -4246,16 +4400,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4264,13 +4418,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4279,13 +4433,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4294,13 +4448,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4309,13 +4463,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4324,13 +4478,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4339,13 +4493,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4354,13 +4508,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4369,13 +4523,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
@@ -4384,13 +4538,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4399,13 +4553,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E12" s="12"/>
     </row>
@@ -4415,13 +4569,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="7"/>
@@ -4432,13 +4586,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>58</v>
-      </c>
       <c r="D14" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E14" s="12"/>
     </row>
@@ -4448,13 +4602,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>59</v>
-      </c>
       <c r="D15" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" s="12"/>
     </row>
@@ -4464,13 +4618,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="10"/>
@@ -4481,13 +4635,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C17" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>75</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="E17" s="12"/>
     </row>
@@ -4497,13 +4651,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E18" s="12"/>
     </row>
@@ -4513,13 +4667,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E19" s="12"/>
     </row>
@@ -4529,13 +4683,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E20" s="12"/>
     </row>
@@ -4545,17 +4699,17 @@
         <v>20</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C21" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>82</v>
       </c>
       <c r="E21" s="12"/>
       <c r="F21" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -4766,13 +4920,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -4781,10 +4935,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>84</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>86</v>
       </c>
       <c r="D3" s="16"/>
     </row>
@@ -5538,34 +5692,34 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -5587,7 +5741,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test plan: add check that wps is automatically switching down after 2 minutes from the moment wps button was pressed
</commit_message>
<xml_diff>
--- a/Test/C780_Binary_Library_Test_Plan.xlsx
+++ b/Test/C780_Binary_Library_Test_Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="V.0.01" sheetId="3" r:id="rId1"/>
@@ -572,7 +572,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="207">
   <si>
     <t>Test ID</t>
   </si>
@@ -1446,6 +1446,15 @@
   <si>
     <t>Use an application with 2 parameters having different hysteresis values. 
 Change the 2 values</t>
+  </si>
+  <si>
+    <t>Test that gme keeps wps active for a limited period of time</t>
+  </si>
+  <si>
+    <t>1. select WPS in web page and check current time</t>
+  </si>
+  <si>
+    <t>1. Wait for more than 2 minutes before pressing button on wifi modem: connection is not possible (wps is no more active)</t>
   </si>
 </sst>
 </file>
@@ -2785,10 +2794,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2912,7 +2921,7 @@
     </row>
     <row r="8" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="21">
-        <f t="shared" ref="A8:A10" si="0">A7+1</f>
+        <f t="shared" ref="A8:A12" si="0">A7+1</f>
         <v>7</v>
       </c>
       <c r="B8" s="24" t="s">
@@ -2955,167 +2964,173 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="B11" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="21">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C12" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D12" s="16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="21">
-        <f>A11+1</f>
-        <v>10</v>
-      </c>
-      <c r="B12" s="24" t="s">
+    <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="21">
+        <f>A12+1</f>
+        <v>12</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C13" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A13" s="21">
-        <f t="shared" ref="A13:A38" si="1">A12+1</f>
-        <v>11</v>
-      </c>
-      <c r="B13" s="23" t="s">
+    <row r="14" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="21">
+        <f t="shared" ref="A14:A39" si="1">A13+1</f>
+        <v>13</v>
+      </c>
+      <c r="B14" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C14" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D14" s="16" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="21">
-        <f t="shared" si="1"/>
-        <v>12</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="21">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>149</v>
+        <v>15</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>119</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="21">
         <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>150</v>
+        <v>16</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>149</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="21">
         <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>154</v>
+      </c>
       <c r="E18" s="12"/>
-      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="23"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
       <c r="E19" s="12"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="23"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="17"/>
       <c r="E20" s="12"/>
     </row>
     <row r="21" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="23"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="12"/>
-      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="23"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="17"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="12"/>
+      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" s="23"/>
       <c r="C23" s="18"/>
@@ -3125,9 +3140,9 @@
     <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21">
         <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-      <c r="B24" s="25"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="23"/>
       <c r="C24" s="18"/>
       <c r="D24" s="17"/>
       <c r="E24" s="12"/>
@@ -3135,9 +3150,9 @@
     <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21">
         <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="B25" s="23"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="25"/>
       <c r="C25" s="18"/>
       <c r="D25" s="17"/>
       <c r="E25" s="12"/>
@@ -3145,88 +3160,88 @@
     <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="21">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="18"/>
       <c r="D26" s="17"/>
       <c r="E26" s="12"/>
     </row>
-    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21">
         <f t="shared" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="B27" s="25"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="23"/>
       <c r="C27" s="18"/>
       <c r="D27" s="17"/>
-      <c r="E27" s="13"/>
-    </row>
-    <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21">
         <f t="shared" si="1"/>
-        <v>26</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="12"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="13"/>
     </row>
     <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21">
         <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="B29" s="24"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="23"/>
       <c r="C29" s="19"/>
-      <c r="D29" s="16"/>
+      <c r="D29" s="18"/>
       <c r="E29" s="12"/>
     </row>
     <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21">
         <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="17"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="24"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="16"/>
       <c r="E30" s="12"/>
     </row>
     <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" s="23"/>
       <c r="C31" s="18"/>
       <c r="D31" s="17"/>
       <c r="E31" s="12"/>
-      <c r="F31" s="10"/>
     </row>
     <row r="32" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="18"/>
       <c r="D32" s="17"/>
       <c r="E32" s="12"/>
+      <c r="F32" s="10"/>
     </row>
     <row r="33" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="23"/>
-      <c r="C33" s="16"/>
+      <c r="C33" s="18"/>
       <c r="D33" s="17"/>
       <c r="E33" s="12"/>
     </row>
     <row r="34" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" s="23"/>
       <c r="C34" s="16"/>
@@ -3236,36 +3251,36 @@
     <row r="35" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="16"/>
       <c r="D35" s="17"/>
       <c r="E35" s="12"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21">
         <f t="shared" si="1"/>
-        <v>34</v>
-      </c>
-      <c r="B36" s="24"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="23"/>
       <c r="C36" s="16"/>
       <c r="D36" s="17"/>
+      <c r="E36" s="12"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="21">
         <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="F37" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="24"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="17"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="21">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B38" s="26"/>
       <c r="C38" s="11"/>
@@ -3274,17 +3289,27 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="21">
-        <v>33</v>
-      </c>
-      <c r="B39" s="23"/>
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="B39" s="26"/>
       <c r="C39" s="11"/>
       <c r="D39" s="11"/>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E40" s="15"/>
+      <c r="A40" s="21">
+        <v>33</v>
+      </c>
+      <c r="B40" s="23"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E41" s="15"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1 E13:E1048576">
+  <conditionalFormatting sqref="E1 E14:E1048576">
     <cfRule type="containsText" dxfId="29" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
@@ -3300,7 +3325,7 @@
       <formula>NOT(ISERROR(SEARCH("FAIL",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E12">
+  <conditionalFormatting sqref="E2:E13">
     <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
     </cfRule>
@@ -3321,7 +3346,7 @@
           <x14:formula1>
             <xm:f>Support!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E367</xm:sqref>
+          <xm:sqref>E2:E368</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3875,7 +3900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added some test and a new section for security test
</commit_message>
<xml_diff>
--- a/Test/C780_Binary_Library_Test_Plan.xlsx
+++ b/Test/C780_Binary_Library_Test_Plan.xlsx
@@ -9,26 +9,28 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="V.0.01" sheetId="3" r:id="rId1"/>
     <sheet name="Instruction_Legenda" sheetId="5" r:id="rId2"/>
     <sheet name="HW_TEST" sheetId="13" r:id="rId3"/>
     <sheet name="Miscellaneous" sheetId="14" r:id="rId4"/>
-    <sheet name="rtc configuration" sheetId="12" r:id="rId5"/>
-    <sheet name="wifi configuration" sheetId="6" r:id="rId6"/>
-    <sheet name="mqtt communication" sheetId="7" r:id="rId7"/>
-    <sheet name="modbus communication" sheetId="8" r:id="rId8"/>
-    <sheet name="CBOR encoding" sheetId="10" r:id="rId9"/>
-    <sheet name="default config" sheetId="9" r:id="rId10"/>
-    <sheet name="gsm configuration" sheetId="11" r:id="rId11"/>
-    <sheet name="Support" sheetId="4" r:id="rId12"/>
+    <sheet name="Security_Related" sheetId="15" r:id="rId5"/>
+    <sheet name="rtc configuration" sheetId="12" r:id="rId6"/>
+    <sheet name="wifi configuration" sheetId="6" r:id="rId7"/>
+    <sheet name="mqtt communication" sheetId="7" r:id="rId8"/>
+    <sheet name="modbus communication" sheetId="8" r:id="rId9"/>
+    <sheet name="CBOR encoding" sheetId="10" r:id="rId10"/>
+    <sheet name="default config" sheetId="9" r:id="rId11"/>
+    <sheet name="gsm configuration" sheetId="11" r:id="rId12"/>
+    <sheet name="Support" sheetId="4" r:id="rId13"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'mqtt communication'!$A$1:$F$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'V.0.01'!$A$1:$F$337</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -108,6 +110,73 @@
 </file>
 
 <file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alessandro Bilato</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Brief description of the scope of the test
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Test preconditions
+ie. Status of the connection, status of the monitored device etc.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Expected Result
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">if something was wrong a brief explanation of what happened
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Alessandro Bilato</author>
@@ -711,7 +780,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="244">
   <si>
     <t>Test ID</t>
   </si>
@@ -1649,27 +1718,102 @@
 Configured / Connected to Internet</t>
   </si>
   <si>
-    <t>Button Test  - reset</t>
-  </si>
-  <si>
-    <t>Button Test  - 
-restore default communication parameters</t>
-  </si>
-  <si>
-    <t>1. the GME reboot itself and reconnect to the cloud</t>
-  </si>
-  <si>
-    <t>1. GME powered
-2. configured to access the cloud
-3. press the button &lt;5sec.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. GME powered
-2. configure to access the cloud
-2. press the button &gt;10sec. Wait the fast blinking press the button again </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. the GME reboot itself and wait for the configuration </t>
+    <t>Verify if the official CAREL SIM connect to our 
+server</t>
+  </si>
+  <si>
+    <t>1. the IMEI of the device under test is registered on CAREL cloud
+2, power on the system</t>
+  </si>
+  <si>
+    <t>Through the RED portal or through the test program in a short time
+&lt; 2min you will see the Hello message from the GME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that the device is able to connect to an AP
+with hidden SSID </t>
+  </si>
+  <si>
+    <t>1. a test AP connected to the internet 
+     configured as follow :
+   - SSID "TEST_AP" with hidden SSID
+   - Security : WPA
+   - Password : "12345678"
+   - DHCP on
+2. a device with all the connections parameter already configured as above</t>
+  </si>
+  <si>
+    <t>a. the system do not accept an empty pwd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if the configuration page accept only valid fields
+a. empty AP pwd not allowed
+b. </t>
+  </si>
+  <si>
+    <t>WatchDog test</t>
+  </si>
+  <si>
+    <t>0. the test program MqttClientSimulatorBinary.exe is running and with the 
+MAC/IMEI number set to point to the device under test
+1. configure the GME to access the Internet through a suitable AP
+2. make sure that the MAC of the GME is already registered in the cloud
+3. when you see the "hello" message wait 2min 
+4. On MqttClientSimulatorBinary press button "trig WD"</t>
+  </si>
+  <si>
+    <t>1. in a short time you will see the GME that reboot itself</t>
+  </si>
+  <si>
+    <t>1. GME configured and running
+2. try to upload via OTA an unsigned FW</t>
+  </si>
+  <si>
+    <t>1. The GME restart with original FW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only signed FW  is accepted </t>
+  </si>
+  <si>
+    <t>Update certificate via cable</t>
+  </si>
+  <si>
+    <t>1. GME configured and running
+2. use the update SPIFFS batch to upload a new image with new certificate</t>
+  </si>
+  <si>
+    <t>1. verifiy that the system continua to work right 
+2. verify that the 3 time update counter doesn't increment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated FW via cable </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WARNING! WARNING! WARNING!
+This test must be done only 3 times on a device, after that the only possibility to upload is through OTA. So perform it as one of the last test.
+1. GME configured and running
+2. connect a USB/TTL 5V adapter to the TTL port
+3. press the button and power on  
+4. use the upgrade batch file to install a new FW
+5. power off and on again 
+</t>
+  </si>
+  <si>
+    <t>1. verify that the new FW is installed and running properly</t>
+  </si>
+  <si>
+    <t>1. GME configured and running 
+2. power off the GME
+3. connect a USB/TTL 5V adapter to the TTL port
+3. press the button and power on  
+4. use the memory dump batch file to dump the GME memory</t>
+  </si>
+  <si>
+    <t>1. verify that the plain text FW is not present in the memory, indirectly this confirm that the flash encryption mechanism was triggered properly.</t>
+  </si>
+  <si>
+    <t>Verify that the encryption mechanism is running
+properly (TBC dipende dal tipo di chiave usiamo )</t>
   </si>
 </sst>
 </file>
@@ -1874,350 +2018,7 @@
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="76">
     <dxf>
       <fill>
         <patternFill>
@@ -2568,6 +2369,188 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2586,7 +2569,8 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="V.0.01"/>
-      <sheetName val="HW_Test"/>
+      <sheetName val="Instruction_Legenda"/>
+      <sheetName val="HW_TEST"/>
       <sheetName val="Miscellaneous"/>
       <sheetName val="rtc configuration"/>
       <sheetName val="wifi configuration"/>
@@ -2595,7 +2579,6 @@
       <sheetName val="CBOR encoding"/>
       <sheetName val="default config"/>
       <sheetName val="gsm configuration"/>
-      <sheetName val="Instruction_Legenda"/>
       <sheetName val="Support"/>
     </sheetNames>
     <sheetDataSet>
@@ -2977,13 +2960,13 @@
   </sheetData>
   <autoFilter ref="A1:F337"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="98" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="75" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="74" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="73" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3010,13 +2993,13 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40" style="27" customWidth="1"/>
+    <col min="2" max="2" width="61.33203125" style="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="67.33203125" customWidth="1"/>
     <col min="4" max="4" width="56" customWidth="1"/>
     <col min="5" max="5" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
@@ -3043,206 +3026,322 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>83</v>
+      <c r="B2" s="23" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>82</v>
+      <c r="B3" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="16"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
         <f t="shared" ref="A5:A33" si="0">A4+1</f>
         <v>4</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="21">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="21">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-    </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="B12" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="E12" s="12"/>
     </row>
-    <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="21">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
+      <c r="B13" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="E13" s="12"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="21">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="17"/>
+      <c r="B14" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="E14" s="12"/>
     </row>
-    <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="21">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
+      <c r="B15" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="E15" s="12"/>
     </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
+      <c r="B16" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>74</v>
+      </c>
       <c r="E16" s="12"/>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="21">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="17"/>
+      <c r="B17" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>75</v>
+      </c>
       <c r="E17" s="12"/>
     </row>
-    <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="21">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="17"/>
+      <c r="B18" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>76</v>
+      </c>
       <c r="E18" s="12"/>
     </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="21">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="17"/>
+      <c r="B19" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>77</v>
+      </c>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="21">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17"/>
+      <c r="B20" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="17"/>
+      <c r="B21" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>80</v>
+      </c>
       <c r="E21" s="12"/>
+      <c r="F21" s="6" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21">
@@ -3377,18 +3476,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="66" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="20" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3414,7 +3513,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3447,21 +3546,31 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="16"/>
+      <c r="B3" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>84</v>
+      </c>
       <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -3771,18 +3880,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="62" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="15" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="59" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3804,6 +3913,406 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="27" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="21">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="21">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="21">
+        <f t="shared" ref="A5:A33" si="0">A4+1</f>
+        <v>4</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="21">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="24"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="21">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="21">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="21">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="21">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="25"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="21">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="21">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="23"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="12"/>
+    </row>
+    <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="21">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="23"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="21">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="21">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="23"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="12"/>
+    </row>
+    <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="21">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="23"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="21">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="24"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="21">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="21">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="26"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="21">
+        <v>33</v>
+      </c>
+      <c r="B34" s="23"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E35" s="15"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:E1048576">
+    <cfRule type="containsText" dxfId="13" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Support!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E362</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -3918,7 +4427,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4302,62 +4811,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1 E7:E1048576">
-    <cfRule type="containsText" dxfId="58" priority="16" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="72" priority="16" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="17" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="71" priority="17" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="19" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="70" priority="19" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="containsText" dxfId="55" priority="18" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="69" priority="18" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="51" priority="10" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="68" priority="10" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="11" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="67" priority="11" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="12" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="66" priority="12" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2 E4">
-    <cfRule type="containsText" dxfId="45" priority="7" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="65" priority="7" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="8" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="64" priority="8" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="9" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="63" priority="9" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="39" priority="4" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="6" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="59" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="3" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4388,8 +4897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4462,35 +4971,29 @@
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>226</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>227</v>
-      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
@@ -4763,40 +5266,40 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1 E8:E1048576">
-    <cfRule type="containsText" dxfId="27" priority="19" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="56" priority="19" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="20" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="55" priority="20" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="54" priority="22" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="53" priority="21" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E7">
-    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="52" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="51" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="50" priority="6" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="49" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="48" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="47" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4827,6 +5330,443 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" style="27" customWidth="1"/>
+    <col min="3" max="3" width="67.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="21">
+        <f t="shared" ref="A3:A32" si="0">A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="144" x14ac:dyDescent="0.3">
+      <c r="A4" s="21">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="21">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>241</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="21">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="21">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="21">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="21">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+    </row>
+    <row r="11" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="25"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="21">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="24"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="21">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="12"/>
+    </row>
+    <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="21">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="23"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="21">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="23"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="21">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="21">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="23"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="12"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="21">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="24"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="21">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="26"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="21">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="21">
+        <v>33</v>
+      </c>
+      <c r="B33" s="23"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="15"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1 E8:E1048576">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",F4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5:E7">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E4">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="BLOCKING">
+      <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Support!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E8:E361</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Support!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F34"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
@@ -5194,29 +6134,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1 E5:E1048576">
-    <cfRule type="containsText" dxfId="95" priority="4" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="46" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="45" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="7" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="44" priority="7" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="containsText" dxfId="92" priority="6" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="43" priority="6" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4">
-    <cfRule type="containsText" dxfId="91" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="42" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="41" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="3" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="40" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5237,12 +6177,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5291,7 +6231,7 @@
     </row>
     <row r="3" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A24" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -5306,7 +6246,7 @@
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
-        <f>A3+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="23" t="s">
@@ -5321,7 +6261,7 @@
     </row>
     <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="23" t="s">
@@ -5336,7 +6276,7 @@
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="23" t="s">
@@ -5351,7 +6291,7 @@
     </row>
     <row r="7" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="23" t="s">
@@ -5366,7 +6306,7 @@
     </row>
     <row r="8" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A8" s="21">
-        <f t="shared" ref="A8:A12" si="0">A7+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="24" t="s">
@@ -5379,212 +6319,209 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="24" t="s">
+        <v>225</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="21">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C10" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D10" s="16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="21">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="24" t="s">
+    <row r="11" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C11" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D11" s="16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="21">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="24" t="s">
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="21">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="24" t="s">
         <v>204</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C12" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D12" s="16" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="21">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="24" t="s">
+    <row r="13" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="21">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C13" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D13" s="16" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="21">
-        <f>A12+1</f>
-        <v>12</v>
-      </c>
-      <c r="B13" s="24" t="s">
+    <row r="14" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="21">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C14" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D14" s="16" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A14" s="21">
-        <f t="shared" ref="A14:A39" si="1">A13+1</f>
-        <v>13</v>
-      </c>
-      <c r="B14" s="23" t="s">
+    <row r="15" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="21">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C15" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D15" s="16" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="21">
-        <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="21">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C17" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D17" s="16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="21">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="E18" s="12"/>
+      <c r="B18" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="23"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="12"/>
-      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="23"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
       <c r="E20" s="12"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="23"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
       <c r="E21" s="12"/>
     </row>
     <row r="22" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="23"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
       <c r="E22" s="12"/>
-      <c r="F22" s="10"/>
     </row>
     <row r="23" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="23"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="17"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="12"/>
+      <c r="F23" s="10"/>
     </row>
     <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="23"/>
@@ -5594,10 +6531,10 @@
     </row>
     <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A25:A26" si="1">A24+1</f>
         <v>24</v>
       </c>
-      <c r="B25" s="25"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="18"/>
       <c r="D25" s="17"/>
       <c r="E25" s="12"/>
@@ -5607,14 +6544,14 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B26" s="23"/>
+      <c r="B26" s="25"/>
       <c r="C26" s="18"/>
       <c r="D26" s="17"/>
       <c r="E26" s="12"/>
     </row>
     <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A27:A42" si="2">A26+1</f>
         <v>26</v>
       </c>
       <c r="B27" s="23"/>
@@ -5622,80 +6559,80 @@
       <c r="D27" s="17"/>
       <c r="E27" s="12"/>
     </row>
-    <row r="28" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="B28" s="25"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="18"/>
       <c r="D28" s="17"/>
-      <c r="E28" s="13"/>
-    </row>
-    <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="12"/>
+    </row>
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="12"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="13"/>
     </row>
     <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="B30" s="24"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="19"/>
-      <c r="D30" s="16"/>
+      <c r="D30" s="18"/>
       <c r="E30" s="12"/>
     </row>
     <row r="31" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="17"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="16"/>
       <c r="E31" s="12"/>
     </row>
     <row r="32" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="18"/>
       <c r="D32" s="17"/>
       <c r="E32" s="12"/>
-      <c r="F32" s="10"/>
     </row>
     <row r="33" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="B33" s="23"/>
       <c r="C33" s="18"/>
       <c r="D33" s="17"/>
       <c r="E33" s="12"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33</v>
       </c>
       <c r="B34" s="23"/>
-      <c r="C34" s="16"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="17"/>
       <c r="E34" s="12"/>
     </row>
     <row r="35" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="B35" s="23"/>
@@ -5705,7 +6642,7 @@
     </row>
     <row r="36" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35</v>
       </c>
       <c r="B36" s="23"/>
@@ -5713,28 +6650,28 @@
       <c r="D36" s="17"/>
       <c r="E36" s="12"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="B37" s="24"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="16"/>
       <c r="D37" s="17"/>
+      <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="F38" s="9"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="17"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="B39" s="26"/>
@@ -5744,40 +6681,55 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="21">
-        <v>33</v>
-      </c>
-      <c r="B40" s="23"/>
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="B40" s="26"/>
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
+      <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E41" s="15"/>
+      <c r="A41" s="21">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="B41" s="23"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="21">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="E42" s="15"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E1 E14:E1048576">
-    <cfRule type="containsText" dxfId="88" priority="4" operator="containsText" text="BLOCKING">
+  <conditionalFormatting sqref="E1 E15:E1048576">
+    <cfRule type="containsText" dxfId="39" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="38" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="7" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="37" priority="7" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="containsText" dxfId="85" priority="6" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="36" priority="6" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E13">
-    <cfRule type="containsText" dxfId="84" priority="1" operator="containsText" text="BLOCKING">
+  <conditionalFormatting sqref="E2:E14">
+    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="3" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5791,7 +6743,7 @@
           <x14:formula1>
             <xm:f>Support!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E368</xm:sqref>
+          <xm:sqref>E2:E369</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -5799,12 +6751,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6190,7 +7142,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="24"/>
-      <c r="C25" s="19"/>
+      <c r="C25" s="16"/>
       <c r="D25" s="16"/>
       <c r="E25" s="12"/>
     </row>
@@ -6200,8 +7152,8 @@
         <v>24</v>
       </c>
       <c r="B26" s="23"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="17"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
       <c r="E26" s="12"/>
     </row>
     <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
@@ -6210,8 +7162,6 @@
         <v>25</v>
       </c>
       <c r="B27" s="23"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="17"/>
       <c r="E27" s="12"/>
       <c r="F27" s="10"/>
     </row>
@@ -6296,30 +7246,31 @@
       <c r="E36" s="15"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F36"/>
   <conditionalFormatting sqref="E1:E2 E4:E1048576">
-    <cfRule type="containsText" dxfId="81" priority="4" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="32" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="31" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="7" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="30" priority="7" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="78" priority="6" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="29" priority="6" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="containsText" dxfId="77" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="28" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="27" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="3" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="26" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6341,7 +7292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
@@ -6794,18 +7745,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="74" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="23" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="containsText" dxfId="71" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6825,524 +7776,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.33203125" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.33203125" customWidth="1"/>
-    <col min="4" max="4" width="56" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" s="21">
-        <v>1</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="21">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="21">
-        <f>A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="21">
-        <f t="shared" ref="A5:A33" si="0">A4+1</f>
-        <v>4</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="21">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="21">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="21">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="21">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="21">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="21">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="21">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="21">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="21">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="21">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="12"/>
-    </row>
-    <row r="16" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="21">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="21">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="21">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="21">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="1:6" s="6" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="21">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="1:6" s="6" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="21">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="21">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="13"/>
-    </row>
-    <row r="23" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="21">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="12"/>
-    </row>
-    <row r="25" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="21">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="21">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="28" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="21">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="12"/>
-    </row>
-    <row r="29" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="21">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="21">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="12"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="21">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="17"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="21">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="F32" s="9"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="21">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="F33" s="9"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="21">
-        <v>33</v>
-      </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E35" s="15"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="70" priority="1" operator="containsText" text="BLOCKING">
-      <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="2" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="67" priority="3" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Support!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E362</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added new wireless test
</commit_message>
<xml_diff>
--- a/Test/C780_Binary_Library_Test_Plan.xlsx
+++ b/Test/C780_Binary_Library_Test_Plan.xlsx
@@ -805,7 +805,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="255">
   <si>
     <t>Test ID</t>
   </si>
@@ -1835,10 +1835,6 @@
 - the GME restore the connection as soon Internet is reacheable again</t>
   </si>
   <si>
-    <t xml:space="preserve">WiFi - simply use a router and detach the connection with the provider
-2G - use a shielded dummy load on the antenna connector </t>
-  </si>
-  <si>
     <t>WiFi - Check that the GME connect only to an AP that have the right security level (WPA2)</t>
   </si>
   <si>
@@ -1862,6 +1858,27 @@
   </si>
   <si>
     <t>Initial version</t>
+  </si>
+  <si>
+    <t>WiFi - Check that GME connect to an AP also if this is not initially available.</t>
+  </si>
+  <si>
+    <t>- GME configured and powered on
+- Test AP configured but powered off</t>
+  </si>
+  <si>
+    <t>The GME will connect to the AP within 2 min starting from the availability 
+of the test AP</t>
+  </si>
+  <si>
+    <t>The scope of this test is to verify the robustness of the system after a global
+power fail, where every device have your own power up time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WiFi - simply use a router and detach the connection with the provider
+2G - use a shielded dummy load on the antenna connector 
+Pass after fix commit #763
+</t>
   </si>
 </sst>
 </file>
@@ -2099,112 +2116,7 @@
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="91">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="82">
     <dxf>
       <fill>
         <patternFill>
@@ -2342,6 +2254,48 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3067,10 +3021,10 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="41" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
@@ -3079,10 +3033,10 @@
     </row>
     <row r="2" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C2" s="40"/>
       <c r="D2" s="40"/>
@@ -3125,13 +3079,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="90" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="81" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="80" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="79" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3606,18 +3560,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="13" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="containsText" dxfId="27" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4127,18 +4081,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="26" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4531,18 +4485,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4931,18 +4885,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5462,62 +5416,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1 E7:E1048576">
-    <cfRule type="containsText" dxfId="87" priority="16" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="78" priority="16" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="17" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="77" priority="17" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="19" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="76" priority="19" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="containsText" dxfId="84" priority="18" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="75" priority="18" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="83" priority="10" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="74" priority="10" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="11" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="12" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="72" priority="12" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2 E4">
-    <cfRule type="containsText" dxfId="80" priority="7" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="71" priority="7" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="8" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="70" priority="8" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="9" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="69" priority="9" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="containsText" dxfId="77" priority="4" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="68" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="67" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="6" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="66" priority="6" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="containsText" dxfId="74" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="3" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5917,40 +5871,40 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1 E8:E1048576">
-    <cfRule type="containsText" dxfId="71" priority="19" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="62" priority="19" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="20" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="61" priority="20" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="22" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="60" priority="22" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="containsText" dxfId="68" priority="21" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="59" priority="21" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E7">
-    <cfRule type="containsText" dxfId="67" priority="4" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="58" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="57" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="6" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="56" priority="6" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4">
-    <cfRule type="containsText" dxfId="64" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="55" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="54" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="3" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="53" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6354,40 +6308,40 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1 E8:E1048576">
-    <cfRule type="containsText" dxfId="61" priority="7" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="52" priority="7" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="8" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="51" priority="8" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="10" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="50" priority="10" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="containsText" dxfId="58" priority="9" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="49" priority="9" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E7">
-    <cfRule type="containsText" dxfId="57" priority="4" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="48" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="47" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="6" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="46" priority="6" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4">
-    <cfRule type="containsText" dxfId="54" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="45" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="44" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="3" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="43" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6785,29 +6739,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1 E5:E1048576">
-    <cfRule type="containsText" dxfId="51" priority="4" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="42" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="41" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="7" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="40" priority="7" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="39" priority="6" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E4">
-    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="38" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="36" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7358,29 +7312,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1 E15:E1048576">
-    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="35" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="7" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="33" priority="7" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="containsText" dxfId="41" priority="6" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F7)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E14">
-    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="31" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="30" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="3" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="29" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7406,8 +7360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7439,7 +7393,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="35" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" s="35" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="33">
         <v>1</v>
       </c>
@@ -7447,7 +7401,7 @@
         <v>240</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D2" s="36" t="s">
         <v>241</v>
@@ -7456,7 +7410,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="35" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -7464,24 +7418,38 @@
         <v>2</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C3" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="D3" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="D3" s="34" t="s">
-        <v>246</v>
-      </c>
-      <c r="E3" s="34"/>
+      <c r="E3" s="34" t="s">
+        <v>7</v>
+      </c>
       <c r="F3" s="34"/>
     </row>
-    <row r="4" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+    <row r="4" spans="1:6" s="35" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="33">
+        <v>3</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>251</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="5" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33"/>
@@ -8709,24 +8677,24 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1">
-    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="28" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="27" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="26" priority="6" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E40">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="25" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="23" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9245,29 +9213,29 @@
   </sheetData>
   <autoFilter ref="A1:F36"/>
   <conditionalFormatting sqref="E1:E2 E4:E1048576">
-    <cfRule type="containsText" dxfId="37" priority="4" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="22" priority="4" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="5" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="7" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="34" priority="6" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="19" priority="6" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="BLOCKING">
+    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="BLOCKING">
       <formula>NOT(ISERROR(SEARCH("BLOCKING",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="FAIL">
+    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="FAIL">
       <formula>NOT(ISERROR(SEARCH("FAIL",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="3" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",E3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
empty the result cells
</commit_message>
<xml_diff>
--- a/Test/C780_Binary_Library_Test_Plan.xlsx
+++ b/Test/C780_Binary_Library_Test_Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_His." sheetId="3" r:id="rId1"/>
@@ -805,7 +805,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="259">
   <si>
     <t>Test ID</t>
   </si>
@@ -1879,6 +1879,22 @@
 2G - use a shielded dummy load on the antenna connector 
 Pass after fix commit #763
 </t>
+  </si>
+  <si>
+    <t>WiFi - Check that GME reconnect to an AP initially available and after 
+not reachable or powered off</t>
+  </si>
+  <si>
+    <t>- GME configured and connected to the internet 
+- AP powered off / powered on again</t>
+  </si>
+  <si>
+    <t>The GME will reconnect to the AP within 2 min starting from the availability 
+of the test AP</t>
+  </si>
+  <si>
+    <t>Led status Wifi - case 4
+Configured / NOT Connected to Internet</t>
   </si>
 </sst>
 </file>
@@ -3004,7 +3020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
@@ -5032,7 +5048,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5078,9 +5094,6 @@
       <c r="D2" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
@@ -5096,9 +5109,6 @@
       <c r="D3" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
@@ -5123,9 +5133,6 @@
       <c r="D5" s="16" t="s">
         <v>205</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
@@ -5140,9 +5147,6 @@
       </c>
       <c r="D6" s="16" t="s">
         <v>208</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -5503,7 +5507,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5576,29 +5580,31 @@
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C6" s="16" t="s">
         <v>226</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D6" s="16" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="21">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
@@ -5935,7 +5941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -7360,8 +7366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7451,16 +7457,28 @@
         <v>253</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
+    <row r="5" spans="1:6" s="35" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="33">
+        <v>4</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>257</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>7</v>
+      </c>
       <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="33"/>
+      <c r="A6" s="33">
+        <v>5</v>
+      </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>

</xml_diff>